<commit_message>
added results of jp2
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
@@ -15,7 +15,7 @@
     <sheet name="mpeg4" sheetId="8" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="19">
   <si>
     <t>original size</t>
   </si>
@@ -62,11 +62,32 @@
   <si>
     <t>qscale</t>
   </si>
+  <si>
+    <t>res</t>
+  </si>
+  <si>
+    <t>0.000000</t>
+  </si>
+  <si>
+    <t>0.324074</t>
+  </si>
+  <si>
+    <t>0.648148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000000 </t>
+  </si>
+  <si>
+    <t>0.787037</t>
+  </si>
+  <si>
+    <t>jp2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,7 +122,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -117,9 +138,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -161,6 +182,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -381,7 +403,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D285-4029-9E0F-22CD3577BBD4}"/>
             </c:ext>
@@ -548,7 +570,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D285-4029-9E0F-22CD3577BBD4}"/>
             </c:ext>
@@ -787,11 +809,227 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D285-4029-9E0F-22CD3577BBD4}"/>
             </c:ext>
           </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>jp2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$5:$AD$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5276556352696136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8331019161344071</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1150272348606216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4994320333207121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.749271137026239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9291666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.584027777777778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4962531223980013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5751689189189193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9630801687763713</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$5:$AC$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -801,11 +1039,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="301484912"/>
-        <c:axId val="301485568"/>
+        <c:axId val="401205824"/>
+        <c:axId val="401201512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="301484912"/>
+        <c:axId val="401205824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,12 +1114,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301485568"/>
+        <c:crossAx val="401201512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="301485568"/>
+        <c:axId val="401201512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -952,7 +1190,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301484912"/>
+        <c:crossAx val="401205824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -966,6 +1204,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1028,9 +1267,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1067,6 +1306,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1281,7 +1521,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B252-4A64-A3A5-E10538E0B150}"/>
             </c:ext>
@@ -1454,7 +1694,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B252-4A64-A3A5-E10538E0B150}"/>
             </c:ext>
@@ -1693,11 +1933,227 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B252-4A64-A3A5-E10538E0B150}"/>
             </c:ext>
           </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>jp2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$5:$AD$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5276556352696136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8331019161344071</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1150272348606216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4994320333207121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.749271137026239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9291666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.584027777777778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4962531223980013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5751689189189193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9630801687763713</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$5:$AC$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1707,11 +2163,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="387121648"/>
-        <c:axId val="387122632"/>
+        <c:axId val="401205432"/>
+        <c:axId val="401198768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="387121648"/>
+        <c:axId val="401205432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1782,12 +2238,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387122632"/>
+        <c:crossAx val="401198768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="387122632"/>
+        <c:axId val="401198768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1858,7 +2314,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387121648"/>
+        <c:crossAx val="401205432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1872,6 +2328,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1934,9 +2391,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1973,6 +2430,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2181,7 +2639,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DF8D-45A0-8E36-E537B8795729}"/>
             </c:ext>
@@ -2348,7 +2806,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DF8D-45A0-8E36-E537B8795729}"/>
             </c:ext>
@@ -2587,11 +3045,227 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-DF8D-45A0-8E36-E537B8795729}"/>
             </c:ext>
           </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>jp2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$5:$AD$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5276556352696136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8331019161344071</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1150272348606216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4994320333207121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.749271137026239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9291666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.584027777777778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4962531223980013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5751689189189193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9630801687763713</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$5:$AC$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2601,11 +3275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385166744"/>
-        <c:axId val="385164448"/>
+        <c:axId val="401202688"/>
+        <c:axId val="401205040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385166744"/>
+        <c:axId val="401202688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2676,12 +3350,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385164448"/>
+        <c:crossAx val="401205040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385164448"/>
+        <c:axId val="401205040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2752,7 +3426,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385166744"/>
+        <c:crossAx val="401202688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2766,6 +3440,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2828,9 +3503,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2867,6 +3542,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3087,7 +3763,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-612C-4D05-B8AA-CCAD68B49667}"/>
             </c:ext>
@@ -3272,7 +3948,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-612C-4D05-B8AA-CCAD68B49667}"/>
             </c:ext>
@@ -3451,11 +4127,227 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-612C-4D05-B8AA-CCAD68B49667}"/>
             </c:ext>
           </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>JP2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$5:$AD$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5276556352696136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8331019161344071</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1150272348606216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4994320333207121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.749271137026239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9291666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.584027777777778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4962531223980013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5751689189189193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9630801687763713</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$5:$AC$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3465,11 +4357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="384128112"/>
-        <c:axId val="384128768"/>
+        <c:axId val="401203472"/>
+        <c:axId val="401203864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="384128112"/>
+        <c:axId val="401203472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3540,12 +4432,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384128768"/>
+        <c:crossAx val="401203864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="384128768"/>
+        <c:axId val="401203864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3616,7 +4508,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384128112"/>
+        <c:crossAx val="401203472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3630,6 +4522,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3692,9 +4585,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3872,7 +4765,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-49C1-44D4-AFA2-5833A1D8535E}"/>
             </c:ext>
@@ -4045,7 +4938,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-49C1-44D4-AFA2-5833A1D8535E}"/>
             </c:ext>
@@ -4212,11 +5105,227 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-49C1-44D4-AFA2-5833A1D8535E}"/>
             </c:ext>
           </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>JP2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$5:$AD$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5276556352696136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8331019161344071</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1150272348606216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4994320333207121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.749271137026239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9291666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.584027777777778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4962531223980013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5751689189189193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9630801687763713</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$5:$AC$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4226,11 +5335,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="384134672"/>
-        <c:axId val="384134344"/>
+        <c:axId val="418805992"/>
+        <c:axId val="418806384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="384134672"/>
+        <c:axId val="418805992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4301,12 +5410,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384134344"/>
+        <c:crossAx val="418806384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="384134344"/>
+        <c:axId val="418806384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4377,7 +5486,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384134672"/>
+        <c:crossAx val="418805992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4391,6 +5500,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4453,9 +5563,9 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4492,6 +5602,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4760,7 +5871,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3347-428F-8A08-76C3C577EB41}"/>
             </c:ext>
@@ -4999,7 +6110,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3347-428F-8A08-76C3C577EB41}"/>
             </c:ext>
@@ -5238,11 +6349,227 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3347-428F-8A08-76C3C577EB41}"/>
             </c:ext>
           </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>JP2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$5:$AD$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0851553509781358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5276556352696136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8331019161344071</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1150272348606216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4994320333207121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.749271137026239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.054604349838038</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9291666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.584027777777778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4962531223980013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5751689189189193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8688865764828302</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9630801687763713</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.1553398058252426</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$5:$AC$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5252,11 +6579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="388123424"/>
-        <c:axId val="388124736"/>
+        <c:axId val="418810304"/>
+        <c:axId val="418805208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="388123424"/>
+        <c:axId val="418810304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5327,12 +6654,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388124736"/>
+        <c:crossAx val="418805208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="388124736"/>
+        <c:axId val="418805208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5403,7 +6730,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388123424"/>
+        <c:crossAx val="418810304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5417,6 +6744,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8818,7 +10146,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8829,7 +10157,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8840,7 +10168,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8851,7 +10179,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8862,7 +10190,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8873,7 +10201,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8884,13 +10212,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58E8F331-C253-439C-B3D1-3AD22E973ABD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{58E8F331-C253-439C-B3D1-3AD22E973ABD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8917,13 +10245,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3E00430-68ED-4ECB-8768-746562E49869}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E3E00430-68ED-4ECB-8768-746562E49869}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8950,13 +10278,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9A00B3B-1CDE-4762-8D33-2961CAA9EC0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9A00B3B-1CDE-4762-8D33-2961CAA9EC0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8983,13 +10311,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59758313-3158-475B-AA96-AD219374597F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59758313-3158-475B-AA96-AD219374597F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9016,13 +10344,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43CD7BF8-148D-44CF-B0C7-25E2BAF6F3F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{43CD7BF8-148D-44CF-B0C7-25E2BAF6F3F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9049,13 +10377,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:ext cx="9304020" cy="6019800"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BEBACB8-7D85-4E4B-A90B-21C318BEBA6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BEBACB8-7D85-4E4B-A90B-21C318BEBA6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9341,20 +10669,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:W97"/>
+  <dimension ref="B3:AD97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -9365,7 +10693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -9420,8 +10748,23 @@
       <c r="W4" t="s">
         <v>10</v>
       </c>
+      <c r="Z4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -9438,7 +10781,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f>$C$3/E5</f>
+        <f t="shared" ref="G5:G50" si="0">$C$3/E5</f>
         <v>1.1718444878395171</v>
       </c>
       <c r="J5" t="s">
@@ -9457,7 +10800,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <f>$C$3/M5</f>
+        <f t="shared" ref="O5:O36" si="1">$C$3/M5</f>
         <v>1.6804989816700611</v>
       </c>
       <c r="R5" t="s">
@@ -9476,11 +10819,27 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <f>$C$3/U5</f>
+        <f t="shared" ref="W5:W36" si="2">$C$3/U5</f>
         <v>5.0274181264280271</v>
       </c>
+      <c r="Z5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>24332</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD5">
+        <f>$C$3/AB5</f>
+        <v>1.0851553509781358</v>
+      </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -9497,7 +10856,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f>$C$3/E6</f>
+        <f t="shared" si="0"/>
         <v>1.1840358744394619</v>
       </c>
       <c r="J6" t="s">
@@ -9516,7 +10875,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <f>$C$3/M6</f>
+        <f t="shared" si="1"/>
         <v>2.0506368437402922</v>
       </c>
       <c r="R6" t="s">
@@ -9535,11 +10894,27 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <f>$C$3/U6</f>
+        <f t="shared" si="2"/>
         <v>5.0274181264280271</v>
       </c>
+      <c r="Z6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <v>24332</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD6">
+        <f>$C$3/AB6</f>
+        <v>1.0851553509781358</v>
+      </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -9556,7 +10931,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f>$C$3/E7</f>
+        <f t="shared" si="0"/>
         <v>1.3316522089973775</v>
       </c>
       <c r="J7" t="s">
@@ -9575,7 +10950,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <f>$C$3/M7</f>
+        <f t="shared" si="1"/>
         <v>2.5704828660436139</v>
       </c>
       <c r="R7" t="s">
@@ -9594,11 +10969,27 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W7">
-        <f>$C$3/U7</f>
+        <f t="shared" si="2"/>
         <v>7.666666666666667</v>
       </c>
+      <c r="Z7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA7">
+        <v>3</v>
+      </c>
+      <c r="AB7">
+        <v>21896</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7">
+        <f>$C$3/AB7</f>
+        <v>1.2058823529411764</v>
+      </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -9615,7 +11006,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>$C$3/E8</f>
+        <f t="shared" si="0"/>
         <v>1.5237765466297322</v>
       </c>
       <c r="J8" t="s">
@@ -9634,7 +11025,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <f>$C$3/M8</f>
+        <f t="shared" si="1"/>
         <v>3.3764705882352941</v>
       </c>
       <c r="R8" t="s">
@@ -9653,11 +11044,27 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <f>$C$3/U8</f>
+        <f t="shared" si="2"/>
         <v>9.6930983847283407</v>
       </c>
+      <c r="Z8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA8">
+        <v>4</v>
+      </c>
+      <c r="AB8">
+        <v>17284</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8">
+        <f>$C$3/AB8</f>
+        <v>1.5276556352696136</v>
+      </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -9674,7 +11081,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f>$C$3/E9</f>
+        <f t="shared" si="0"/>
         <v>1.7947253942359978</v>
       </c>
       <c r="J9" t="s">
@@ -9693,7 +11100,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <f>$C$3/M9</f>
+        <f t="shared" si="1"/>
         <v>4.661723163841808</v>
       </c>
       <c r="R9" t="s">
@@ -9712,11 +11119,27 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W9">
-        <f>$C$3/U9</f>
+        <f t="shared" si="2"/>
         <v>12.917808219178083</v>
       </c>
+      <c r="Z9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA9">
+        <v>5</v>
+      </c>
+      <c r="AB9">
+        <v>14404</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD9">
+        <f>$C$3/AB9</f>
+        <v>1.8331019161344071</v>
+      </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -9733,7 +11156,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>$C$3/E10</f>
+        <f t="shared" si="0"/>
         <v>2.1901128069011282</v>
       </c>
       <c r="J10" t="s">
@@ -9752,7 +11175,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O10">
-        <f>$C$3/M10</f>
+        <f t="shared" si="1"/>
         <v>6.640845070422535</v>
       </c>
       <c r="R10" t="s">
@@ -9771,11 +11194,27 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W10">
-        <f>$C$3/U10</f>
+        <f t="shared" si="2"/>
         <v>16.66919191919192</v>
       </c>
+      <c r="Z10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA10">
+        <v>6</v>
+      </c>
+      <c r="AB10">
+        <v>12484</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD10">
+        <f>$C$3/AB10</f>
+        <v>2.1150272348606216</v>
+      </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -9792,7 +11231,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f>$C$3/E11</f>
+        <f t="shared" si="0"/>
         <v>2.8637744034707158</v>
       </c>
       <c r="J11" t="s">
@@ -9811,7 +11250,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <f>$C$3/M11</f>
+        <f t="shared" si="1"/>
         <v>9.5805515239477508</v>
       </c>
       <c r="R11" t="s">
@@ -9830,11 +11269,27 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W11">
-        <f>$C$3/U11</f>
+        <f t="shared" si="2"/>
         <v>19.188953488372093</v>
       </c>
+      <c r="Z11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA11">
+        <v>7</v>
+      </c>
+      <c r="AB11">
+        <v>10564</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD11">
+        <f>$C$3/AB11</f>
+        <v>2.4994320333207121</v>
+      </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -9851,7 +11306,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <f>$C$3/E12</f>
+        <f t="shared" si="0"/>
         <v>4.193773824650572</v>
       </c>
       <c r="J12" t="s">
@@ -9870,7 +11325,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O12">
-        <f>$C$3/M12</f>
+        <f t="shared" si="1"/>
         <v>13.838574423480084</v>
       </c>
       <c r="R12" t="s">
@@ -9889,11 +11344,27 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W12">
-        <f>$C$3/U12</f>
+        <f t="shared" si="2"/>
         <v>20.823343848580443</v>
       </c>
+      <c r="Z12" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA12">
+        <v>8</v>
+      </c>
+      <c r="AB12">
+        <v>9604</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD12">
+        <f>$C$3/AB12</f>
+        <v>2.749271137026239</v>
+      </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -9910,7 +11381,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f>$C$3/E13</f>
+        <f t="shared" si="0"/>
         <v>6.8688865764828302</v>
       </c>
       <c r="J13" t="s">
@@ -9929,7 +11400,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O13">
-        <f>$C$3/M13</f>
+        <f t="shared" si="1"/>
         <v>20.125</v>
       </c>
       <c r="R13" t="s">
@@ -9948,11 +11419,27 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W13">
-        <f>$C$3/U13</f>
+        <f t="shared" si="2"/>
         <v>22.300675675675677</v>
       </c>
+      <c r="Z13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA13">
+        <v>9</v>
+      </c>
+      <c r="AB13">
+        <v>8644</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD13">
+        <f>$C$3/AB13</f>
+        <v>3.054604349838038</v>
+      </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -9969,7 +11456,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f>$C$3/E14</f>
+        <f t="shared" si="0"/>
         <v>10.681229773462784</v>
       </c>
       <c r="J14" t="s">
@@ -9988,7 +11475,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O14">
-        <f>$C$3/M14</f>
+        <f t="shared" si="1"/>
         <v>27.735294117647058</v>
       </c>
       <c r="R14" t="s">
@@ -10007,11 +11494,27 @@
         <v>0.64814799999999995</v>
       </c>
       <c r="W14">
-        <f>$C$3/U14</f>
+        <f t="shared" si="2"/>
         <v>23.574999999999999</v>
       </c>
+      <c r="Z14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA14">
+        <v>10</v>
+      </c>
+      <c r="AB14">
+        <v>8644</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD14">
+        <f>$C$3/AB14</f>
+        <v>3.054604349838038</v>
+      </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>2</v>
       </c>
@@ -10028,7 +11531,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <f>$C$3/E15</f>
+        <f t="shared" si="0"/>
         <v>15.568396226415095</v>
       </c>
       <c r="J15" t="s">
@@ -10047,7 +11550,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O15">
-        <f>$C$3/M15</f>
+        <f t="shared" si="1"/>
         <v>36.469613259668506</v>
       </c>
       <c r="R15" t="s">
@@ -10066,11 +11569,27 @@
         <v>1.111111</v>
       </c>
       <c r="W15">
-        <f>$C$3/U15</f>
+        <f t="shared" si="2"/>
         <v>24.722846441947567</v>
       </c>
+      <c r="Z15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA15">
+        <v>15</v>
+      </c>
+      <c r="AB15">
+        <v>6720</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD15">
+        <f>$C$3/AB15</f>
+        <v>3.9291666666666667</v>
+      </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>2</v>
       </c>
@@ -10087,7 +11606,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="G16">
-        <f>$C$3/E16</f>
+        <f t="shared" si="0"/>
         <v>22.003333333333334</v>
       </c>
       <c r="J16" t="s">
@@ -10106,7 +11625,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O16">
-        <f>$C$3/M16</f>
+        <f t="shared" si="1"/>
         <v>46.485915492957744</v>
       </c>
       <c r="R16" t="s">
@@ -10125,11 +11644,27 @@
         <v>1.111111</v>
       </c>
       <c r="W16">
-        <f>$C$3/U16</f>
+        <f t="shared" si="2"/>
         <v>25.585271317829456</v>
       </c>
+      <c r="Z16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA16">
+        <v>20</v>
+      </c>
+      <c r="AB16">
+        <v>5760</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD16">
+        <f>$C$3/AB16</f>
+        <v>4.584027777777778</v>
+      </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -10146,7 +11681,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <f>$C$3/E17</f>
+        <f t="shared" si="0"/>
         <v>31.136792452830189</v>
       </c>
       <c r="J17" t="s">
@@ -10165,7 +11700,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="O17">
-        <f>$C$3/M17</f>
+        <f t="shared" si="1"/>
         <v>58.415929203539825</v>
       </c>
       <c r="R17" t="s">
@@ -10184,11 +11719,27 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W17">
-        <f>$C$3/U17</f>
+        <f t="shared" si="2"/>
         <v>26.404</v>
       </c>
+      <c r="Z17" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA17">
+        <v>25</v>
+      </c>
+      <c r="AB17">
+        <v>4804</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD17">
+        <f>$C$3/AB17</f>
+        <v>5.4962531223980013</v>
+      </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -10205,7 +11756,7 @@
         <v>0.64814799999999995</v>
       </c>
       <c r="G18">
-        <f>$C$3/E18</f>
+        <f t="shared" si="0"/>
         <v>44.904761904761905</v>
       </c>
       <c r="J18" t="s">
@@ -10224,7 +11775,7 @@
         <v>2.0833330000000001</v>
       </c>
       <c r="O18">
-        <f>$C$3/M18</f>
+        <f t="shared" si="1"/>
         <v>72.538461538461533</v>
       </c>
       <c r="R18" t="s">
@@ -10243,11 +11794,27 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W18">
-        <f>$C$3/U18</f>
+        <f t="shared" si="2"/>
         <v>27.164609053497941</v>
       </c>
+      <c r="Z18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA18">
+        <v>30</v>
+      </c>
+      <c r="AB18">
+        <v>4736</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD18">
+        <f>$C$3/AB18</f>
+        <v>5.5751689189189193</v>
+      </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -10264,7 +11831,7 @@
         <v>1.111111</v>
       </c>
       <c r="G19">
-        <f>$C$3/E19</f>
+        <f t="shared" si="0"/>
         <v>55.940677966101696</v>
       </c>
       <c r="J19" t="s">
@@ -10283,7 +11850,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="O19">
-        <f>$C$3/M19</f>
+        <f t="shared" si="1"/>
         <v>88.013333333333335</v>
       </c>
       <c r="R19" t="s">
@@ -10302,11 +11869,27 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W19">
-        <f>$C$3/U19</f>
+        <f t="shared" si="2"/>
         <v>27.852320675105485</v>
       </c>
+      <c r="Z19" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA19">
+        <v>35</v>
+      </c>
+      <c r="AB19">
+        <v>3844</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD19">
+        <f>$C$3/AB19</f>
+        <v>6.8688865764828302</v>
+      </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -10323,7 +11906,7 @@
         <v>1.111111</v>
       </c>
       <c r="G20">
-        <f>$C$3/E20</f>
+        <f t="shared" si="0"/>
         <v>66.676767676767682</v>
       </c>
       <c r="J20" t="s">
@@ -10342,7 +11925,7 @@
         <v>2.5462959999999999</v>
       </c>
       <c r="O20">
-        <f>$C$3/M20</f>
+        <f t="shared" si="1"/>
         <v>106.46774193548387</v>
       </c>
       <c r="R20" t="s">
@@ -10361,11 +11944,27 @@
         <v>1.111111</v>
       </c>
       <c r="W20">
-        <f>$C$3/U20</f>
+        <f t="shared" si="2"/>
         <v>28.452586206896552</v>
       </c>
+      <c r="Z20" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA20">
+        <v>40</v>
+      </c>
+      <c r="AB20">
+        <v>3844</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD20">
+        <f>$C$3/AB20</f>
+        <v>6.8688865764828302</v>
+      </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -10382,7 +11981,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="G21">
-        <f>$C$3/E21</f>
+        <f t="shared" si="0"/>
         <v>79.53012048192771</v>
       </c>
       <c r="J21" t="s">
@@ -10401,7 +12000,7 @@
         <v>4.4444439999999998</v>
       </c>
       <c r="O21">
-        <f>$C$3/M21</f>
+        <f t="shared" si="1"/>
         <v>129.43137254901961</v>
       </c>
       <c r="R21" t="s">
@@ -10420,11 +12019,27 @@
         <v>1.111111</v>
       </c>
       <c r="W21">
-        <f>$C$3/U21</f>
+        <f t="shared" si="2"/>
         <v>29.079295154185022</v>
       </c>
+      <c r="Z21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA21">
+        <v>45</v>
+      </c>
+      <c r="AB21">
+        <v>3844</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD21">
+        <f>$C$3/AB21</f>
+        <v>6.8688865764828302</v>
+      </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -10441,7 +12056,7 @@
         <v>2.2222219999999999</v>
       </c>
       <c r="G22">
-        <f>$C$3/E22</f>
+        <f t="shared" si="0"/>
         <v>94.3</v>
       </c>
       <c r="J22" t="s">
@@ -10460,7 +12075,7 @@
         <v>8.1018519999999992</v>
       </c>
       <c r="O22">
-        <f>$C$3/M22</f>
+        <f t="shared" si="1"/>
         <v>157.16666666666666</v>
       </c>
       <c r="R22" t="s">
@@ -10479,11 +12094,27 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="W22">
-        <f>$C$3/U22</f>
+        <f t="shared" si="2"/>
         <v>29.46875</v>
       </c>
+      <c r="Z22" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA22">
+        <v>50</v>
+      </c>
+      <c r="AB22">
+        <v>3844</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD22">
+        <f>$C$3/AB22</f>
+        <v>6.8688865764828302</v>
+      </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -10500,7 +12131,7 @@
         <v>1.8981479999999999</v>
       </c>
       <c r="G23">
-        <f>$C$3/E23</f>
+        <f t="shared" si="0"/>
         <v>111.88135593220339</v>
       </c>
       <c r="J23" t="s">
@@ -10519,7 +12150,7 @@
         <v>11.898148000000001</v>
       </c>
       <c r="O23">
-        <f>$C$3/M23</f>
+        <f t="shared" si="1"/>
         <v>188.6</v>
       </c>
       <c r="R23" t="s">
@@ -10538,11 +12169,27 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="W23">
-        <f>$C$3/U23</f>
+        <f t="shared" si="2"/>
         <v>30.004545454545454</v>
       </c>
+      <c r="Z23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA23">
+        <v>55</v>
+      </c>
+      <c r="AB23">
+        <v>3844</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD23">
+        <f>$C$3/AB23</f>
+        <v>6.8688865764828302</v>
+      </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2</v>
       </c>
@@ -10559,7 +12206,7 @@
         <v>2.8703699999999999</v>
       </c>
       <c r="G24">
-        <f>$C$3/E24</f>
+        <f t="shared" si="0"/>
         <v>129.43137254901961</v>
       </c>
       <c r="J24" t="s">
@@ -10578,7 +12225,7 @@
         <v>22.222221999999999</v>
       </c>
       <c r="O24">
-        <f>$C$3/M24</f>
+        <f t="shared" si="1"/>
         <v>227.62068965517241</v>
       </c>
       <c r="R24" t="s">
@@ -10597,11 +12244,27 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="W24">
-        <f>$C$3/U24</f>
+        <f t="shared" si="2"/>
         <v>30.419354838709676</v>
       </c>
+      <c r="Z24" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA24">
+        <v>60</v>
+      </c>
+      <c r="AB24">
+        <v>3792</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD24">
+        <f>$C$3/AB24</f>
+        <v>6.9630801687763713</v>
+      </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>2</v>
       </c>
@@ -10618,7 +12281,7 @@
         <v>5.5555560000000002</v>
       </c>
       <c r="G25">
-        <f>$C$3/E25</f>
+        <f t="shared" si="0"/>
         <v>150.02272727272728</v>
       </c>
       <c r="J25" t="s">
@@ -10637,7 +12300,7 @@
         <v>31.435185000000001</v>
       </c>
       <c r="O25">
-        <f>$C$3/M25</f>
+        <f t="shared" si="1"/>
         <v>275.04166666666669</v>
       </c>
       <c r="R25" t="s">
@@ -10656,11 +12319,27 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="W25">
-        <f>$C$3/U25</f>
+        <f t="shared" si="2"/>
         <v>30.845794392523363</v>
       </c>
+      <c r="Z25" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA25">
+        <v>65</v>
+      </c>
+      <c r="AB25">
+        <v>2884</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD25">
+        <f>$C$3/AB25</f>
+        <v>9.1553398058252426</v>
+      </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>2</v>
       </c>
@@ -10677,7 +12356,7 @@
         <v>8.5648149999999994</v>
       </c>
       <c r="G26">
-        <f>$C$3/E26</f>
+        <f t="shared" si="0"/>
         <v>173.71052631578948</v>
       </c>
       <c r="J26" t="s">
@@ -10696,7 +12375,7 @@
         <v>42.546295999999998</v>
       </c>
       <c r="O26">
-        <f>$C$3/M26</f>
+        <f t="shared" si="1"/>
         <v>330.05</v>
       </c>
       <c r="R26" t="s">
@@ -10715,11 +12394,27 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="W26">
-        <f>$C$3/U26</f>
+        <f t="shared" si="2"/>
         <v>31.284360189573459</v>
       </c>
+      <c r="Z26" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA26">
+        <v>70</v>
+      </c>
+      <c r="AB26">
+        <v>2884</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD26">
+        <f>$C$3/AB26</f>
+        <v>9.1553398058252426</v>
+      </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>2</v>
       </c>
@@ -10736,7 +12431,7 @@
         <v>15.092593000000001</v>
       </c>
       <c r="G27">
-        <f>$C$3/E27</f>
+        <f t="shared" si="0"/>
         <v>194.14705882352942</v>
       </c>
       <c r="J27" t="s">
@@ -10755,7 +12450,7 @@
         <v>53.657406999999999</v>
       </c>
       <c r="O27">
-        <f>$C$3/M27</f>
+        <f t="shared" si="1"/>
         <v>366.72222222222223</v>
       </c>
       <c r="R27" t="s">
@@ -10774,11 +12469,27 @@
         <v>1.111111</v>
       </c>
       <c r="W27">
-        <f>$C$3/U27</f>
+        <f t="shared" si="2"/>
         <v>31.583732057416267</v>
       </c>
+      <c r="Z27" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA27">
+        <v>75</v>
+      </c>
+      <c r="AB27">
+        <v>2884</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD27">
+        <f>$C$3/AB27</f>
+        <v>9.1553398058252426</v>
+      </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>2</v>
       </c>
@@ -10795,7 +12506,7 @@
         <v>21.759259</v>
       </c>
       <c r="G28">
-        <f>$C$3/E28</f>
+        <f t="shared" si="0"/>
         <v>227.62068965517241</v>
       </c>
       <c r="J28" t="s">
@@ -10814,7 +12525,7 @@
         <v>66.203704000000002</v>
       </c>
       <c r="O28">
-        <f>$C$3/M28</f>
+        <f t="shared" si="1"/>
         <v>412.5625</v>
       </c>
       <c r="R28" t="s">
@@ -10833,11 +12544,27 @@
         <v>1.8981479999999999</v>
       </c>
       <c r="W28">
-        <f>$C$3/U28</f>
+        <f t="shared" si="2"/>
         <v>31.888888888888889</v>
       </c>
+      <c r="Z28" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA28">
+        <v>80</v>
+      </c>
+      <c r="AB28">
+        <v>2884</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD28">
+        <f>$C$3/AB28</f>
+        <v>9.1553398058252426</v>
+      </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>2</v>
       </c>
@@ -10854,7 +12581,7 @@
         <v>28.101852000000001</v>
       </c>
       <c r="G29">
-        <f>$C$3/E29</f>
+        <f t="shared" si="0"/>
         <v>253.88461538461539</v>
       </c>
       <c r="J29" t="s">
@@ -10873,7 +12600,7 @@
         <v>69.212963000000002</v>
       </c>
       <c r="O29">
-        <f>$C$3/M29</f>
+        <f t="shared" si="1"/>
         <v>440.06666666666666</v>
       </c>
       <c r="R29" t="s">
@@ -10892,11 +12619,27 @@
         <v>1.8981479999999999</v>
       </c>
       <c r="W29">
-        <f>$C$3/U29</f>
+        <f t="shared" si="2"/>
         <v>32.200000000000003</v>
       </c>
+      <c r="Z29" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA29">
+        <v>85</v>
+      </c>
+      <c r="AB29">
+        <v>2884</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD29">
+        <f>$C$3/AB29</f>
+        <v>9.1553398058252426</v>
+      </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>2</v>
       </c>
@@ -10913,7 +12656,7 @@
         <v>32.870370000000001</v>
       </c>
       <c r="G30">
-        <f>$C$3/E30</f>
+        <f t="shared" si="0"/>
         <v>314.33333333333331</v>
       </c>
       <c r="J30" t="s">
@@ -10932,7 +12675,7 @@
         <v>0</v>
       </c>
       <c r="O30">
-        <f>$C$3/M30</f>
+        <f t="shared" si="1"/>
         <v>1.6804989816700611</v>
       </c>
       <c r="R30" t="s">
@@ -10951,11 +12694,27 @@
         <v>2.5462959999999999</v>
       </c>
       <c r="W30">
-        <f>$C$3/U30</f>
+        <f t="shared" si="2"/>
         <v>32.517241379310342</v>
       </c>
+      <c r="Z30" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA30">
+        <v>90</v>
+      </c>
+      <c r="AB30">
+        <v>2884</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD30">
+        <f>$C$3/AB30</f>
+        <v>9.1553398058252426</v>
+      </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>2</v>
       </c>
@@ -10972,7 +12731,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <f>$C$3/E31</f>
+        <f t="shared" si="0"/>
         <v>1.1893693693693694</v>
       </c>
       <c r="J31" t="s">
@@ -10991,7 +12750,7 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <f>$C$3/M31</f>
+        <f t="shared" si="1"/>
         <v>2.0506368437402922</v>
       </c>
       <c r="R31" t="s">
@@ -11010,11 +12769,27 @@
         <v>1.111111</v>
       </c>
       <c r="W31">
-        <f>$C$3/U31</f>
+        <f t="shared" si="2"/>
         <v>32.840796019900495</v>
       </c>
+      <c r="Z31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA31">
+        <v>95</v>
+      </c>
+      <c r="AB31">
+        <v>2884</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD31">
+        <f>$C$3/AB31</f>
+        <v>9.1553398058252426</v>
+      </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>2</v>
       </c>
@@ -11031,7 +12806,7 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <f>$C$3/E32</f>
+        <f t="shared" si="0"/>
         <v>1.2874975619270528</v>
       </c>
       <c r="J32" t="s">
@@ -11050,7 +12825,7 @@
         <v>0</v>
       </c>
       <c r="O32">
-        <f>$C$3/M32</f>
+        <f t="shared" si="1"/>
         <v>2.5704828660436139</v>
       </c>
       <c r="R32" t="s">
@@ -11069,8 +12844,24 @@
         <v>3.3333330000000001</v>
       </c>
       <c r="W32">
-        <f>$C$3/U32</f>
+        <f t="shared" si="2"/>
         <v>33.005000000000003</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA32">
+        <v>100</v>
+      </c>
+      <c r="AB32">
+        <v>2884</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD32">
+        <f>$C$3/AB32</f>
+        <v>9.1553398058252426</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
@@ -11090,7 +12881,7 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <f>$C$3/E33</f>
+        <f t="shared" si="0"/>
         <v>1.4652608213096558</v>
       </c>
       <c r="J33" t="s">
@@ -11109,7 +12900,7 @@
         <v>0</v>
       </c>
       <c r="O33">
-        <f>$C$3/M33</f>
+        <f t="shared" si="1"/>
         <v>3.3764705882352941</v>
       </c>
       <c r="R33" t="s">
@@ -11128,7 +12919,7 @@
         <v>3.0092590000000001</v>
       </c>
       <c r="W33">
-        <f>$C$3/U33</f>
+        <f t="shared" si="2"/>
         <v>33.338383838383841</v>
       </c>
     </row>
@@ -11149,7 +12940,7 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <f>$C$3/E34</f>
+        <f t="shared" si="0"/>
         <v>1.7141002337055311</v>
       </c>
       <c r="J34" t="s">
@@ -11168,7 +12959,7 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <f>$C$3/M34</f>
+        <f t="shared" si="1"/>
         <v>4.661723163841808</v>
       </c>
       <c r="R34" t="s">
@@ -11187,7 +12978,7 @@
         <v>3.0092590000000001</v>
       </c>
       <c r="W34">
-        <f>$C$3/U34</f>
+        <f t="shared" si="2"/>
         <v>33.507614213197968</v>
       </c>
     </row>
@@ -11208,7 +12999,7 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <f>$C$3/E35</f>
+        <f t="shared" si="0"/>
         <v>2.0764391318024535</v>
       </c>
       <c r="J35" t="s">
@@ -11227,7 +13018,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O35">
-        <f>$C$3/M35</f>
+        <f t="shared" si="1"/>
         <v>6.640845070422535</v>
       </c>
       <c r="R35" t="s">
@@ -11246,7 +13037,7 @@
         <v>3.7962959999999999</v>
       </c>
       <c r="W35">
-        <f>$C$3/U35</f>
+        <f t="shared" si="2"/>
         <v>33.851282051282048</v>
       </c>
     </row>
@@ -11267,7 +13058,7 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <f>$C$3/E36</f>
+        <f t="shared" si="0"/>
         <v>2.6670707070707071</v>
       </c>
       <c r="J36" t="s">
@@ -11286,7 +13077,7 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <f>$C$3/M36</f>
+        <f t="shared" si="1"/>
         <v>9.5805515239477508</v>
       </c>
       <c r="R36" t="s">
@@ -11305,7 +13096,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W36">
-        <f>$C$3/U36</f>
+        <f t="shared" si="2"/>
         <v>6.4715686274509805</v>
       </c>
     </row>
@@ -11326,7 +13117,7 @@
         <v>0</v>
       </c>
       <c r="G37">
-        <f>$C$3/E37</f>
+        <f t="shared" si="0"/>
         <v>3.7209695603156709</v>
       </c>
       <c r="J37" t="s">
@@ -11345,7 +13136,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O37">
-        <f>$C$3/M37</f>
+        <f t="shared" ref="O37:O68" si="3">$C$3/M37</f>
         <v>13.838574423480084</v>
       </c>
       <c r="R37" t="s">
@@ -11364,7 +13155,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W37">
-        <f>$C$3/U37</f>
+        <f t="shared" ref="W37:W68" si="4">$C$3/U37</f>
         <v>6.497047244094488</v>
       </c>
     </row>
@@ -11385,7 +13176,7 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <f>$C$3/E38</f>
+        <f t="shared" si="0"/>
         <v>5.6758383490971624</v>
       </c>
       <c r="J38" t="s">
@@ -11404,7 +13195,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O38">
-        <f>$C$3/M38</f>
+        <f t="shared" si="3"/>
         <v>20.125</v>
       </c>
       <c r="R38" t="s">
@@ -11423,7 +13214,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W38">
-        <f>$C$3/U38</f>
+        <f t="shared" si="4"/>
         <v>10.108728943338438</v>
       </c>
     </row>
@@ -11444,7 +13235,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="G39">
-        <f>$C$3/E39</f>
+        <f t="shared" si="0"/>
         <v>8.9202702702702705</v>
       </c>
       <c r="J39" t="s">
@@ -11463,7 +13254,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O39">
-        <f>$C$3/M39</f>
+        <f t="shared" si="3"/>
         <v>27.735294117647058</v>
       </c>
       <c r="R39" t="s">
@@ -11482,7 +13273,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W39">
-        <f>$C$3/U39</f>
+        <f t="shared" si="4"/>
         <v>13.045454545454545</v>
       </c>
     </row>
@@ -11503,7 +13294,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="G40">
-        <f>$C$3/E40</f>
+        <f t="shared" si="0"/>
         <v>13.443991853360489</v>
       </c>
       <c r="J40" t="s">
@@ -11522,7 +13313,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O40">
-        <f>$C$3/M40</f>
+        <f t="shared" si="3"/>
         <v>36.469613259668506</v>
       </c>
       <c r="R40" t="s">
@@ -11541,7 +13332,7 @@
         <v>0.64814799999999995</v>
       </c>
       <c r="W40">
-        <f>$C$3/U40</f>
+        <f t="shared" si="4"/>
         <v>17.145454545454545</v>
       </c>
     </row>
@@ -11562,7 +13353,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="G41">
-        <f>$C$3/E41</f>
+        <f t="shared" si="0"/>
         <v>18.914040114613179</v>
       </c>
       <c r="J41" t="s">
@@ -11581,7 +13372,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O41">
-        <f>$C$3/M41</f>
+        <f t="shared" si="3"/>
         <v>46.485915492957744</v>
       </c>
       <c r="R41" t="s">
@@ -11600,7 +13391,7 @@
         <v>0.64814799999999995</v>
       </c>
       <c r="W41">
-        <f>$C$3/U41</f>
+        <f t="shared" si="4"/>
         <v>21.713815789473685</v>
       </c>
     </row>
@@ -11621,7 +13412,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="G42">
-        <f>$C$3/E42</f>
+        <f t="shared" si="0"/>
         <v>26.404</v>
       </c>
       <c r="J42" t="s">
@@ -11640,7 +13431,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="O42">
-        <f>$C$3/M42</f>
+        <f t="shared" si="3"/>
         <v>58.415929203539825</v>
       </c>
       <c r="R42" t="s">
@@ -11659,7 +13450,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W42">
-        <f>$C$3/U42</f>
+        <f t="shared" si="4"/>
         <v>24.909433962264149</v>
       </c>
     </row>
@@ -11680,7 +13471,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="G43">
-        <f>$C$3/E43</f>
+        <f t="shared" si="0"/>
         <v>35.875</v>
       </c>
       <c r="J43" t="s">
@@ -11699,7 +13490,7 @@
         <v>2.0833330000000001</v>
       </c>
       <c r="O43">
-        <f>$C$3/M43</f>
+        <f t="shared" si="3"/>
         <v>72.538461538461533</v>
       </c>
       <c r="R43" t="s">
@@ -11718,7 +13509,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W43">
-        <f>$C$3/U43</f>
+        <f t="shared" si="4"/>
         <v>27.164609053497941</v>
       </c>
     </row>
@@ -11739,7 +13530,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="G44">
-        <f>$C$3/E44</f>
+        <f t="shared" si="0"/>
         <v>49.261194029850749</v>
       </c>
       <c r="J44" t="s">
@@ -11758,7 +13549,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="O44">
-        <f>$C$3/M44</f>
+        <f t="shared" si="3"/>
         <v>88.013333333333335</v>
       </c>
       <c r="R44" t="s">
@@ -11777,7 +13568,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W44">
-        <f>$C$3/U44</f>
+        <f t="shared" si="4"/>
         <v>28.20940170940171</v>
       </c>
     </row>
@@ -11798,7 +13589,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="G45">
-        <f>$C$3/E45</f>
+        <f t="shared" si="0"/>
         <v>61.691588785046726</v>
       </c>
       <c r="J45" t="s">
@@ -11817,7 +13608,7 @@
         <v>2.5462959999999999</v>
       </c>
       <c r="O45">
-        <f>$C$3/M45</f>
+        <f t="shared" si="3"/>
         <v>106.46774193548387</v>
       </c>
       <c r="R45" t="s">
@@ -11836,7 +13627,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W45">
-        <f>$C$3/U45</f>
+        <f t="shared" si="4"/>
         <v>31.136792452830189</v>
       </c>
     </row>
@@ -11857,7 +13648,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="G46">
-        <f>$C$3/E46</f>
+        <f t="shared" si="0"/>
         <v>74.168539325842701</v>
       </c>
       <c r="J46" t="s">
@@ -11876,7 +13667,7 @@
         <v>4.4444439999999998</v>
       </c>
       <c r="O46">
-        <f>$C$3/M46</f>
+        <f t="shared" si="3"/>
         <v>129.43137254901961</v>
       </c>
       <c r="R46" t="s">
@@ -11895,7 +13686,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W46">
-        <f>$C$3/U46</f>
+        <f t="shared" si="4"/>
         <v>31.583732057416267</v>
       </c>
     </row>
@@ -11916,7 +13707,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="G47">
-        <f>$C$3/E47</f>
+        <f t="shared" si="0"/>
         <v>88.013333333333335</v>
       </c>
       <c r="J47" t="s">
@@ -11935,7 +13726,7 @@
         <v>8.1018519999999992</v>
       </c>
       <c r="O47">
-        <f>$C$3/M47</f>
+        <f t="shared" si="3"/>
         <v>157.16666666666666</v>
       </c>
       <c r="R47" t="s">
@@ -11954,7 +13745,7 @@
         <v>1.111111</v>
       </c>
       <c r="W47">
-        <f>$C$3/U47</f>
+        <f t="shared" si="4"/>
         <v>32.678217821782177</v>
       </c>
     </row>
@@ -11975,7 +13766,7 @@
         <v>2.2222219999999999</v>
       </c>
       <c r="G48">
-        <f>$C$3/E48</f>
+        <f t="shared" si="0"/>
         <v>104.77777777777777</v>
       </c>
       <c r="J48" t="s">
@@ -11994,7 +13785,7 @@
         <v>8.8888890000000007</v>
       </c>
       <c r="O48">
-        <f>$C$3/M48</f>
+        <f t="shared" si="3"/>
         <v>169.25641025641025</v>
       </c>
       <c r="R48" t="s">
@@ -12013,7 +13804,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W48">
-        <f>$C$3/U48</f>
+        <f t="shared" si="4"/>
         <v>35.299465240641709</v>
       </c>
     </row>
@@ -12034,7 +13825,7 @@
         <v>4.1203700000000003</v>
       </c>
       <c r="G49">
-        <f>$C$3/E49</f>
+        <f t="shared" si="0"/>
         <v>124.54716981132076</v>
       </c>
       <c r="J49" t="s">
@@ -12053,7 +13844,7 @@
         <v>11.898148000000001</v>
       </c>
       <c r="O49">
-        <f>$C$3/M49</f>
+        <f t="shared" si="3"/>
         <v>188.6</v>
       </c>
       <c r="R49" t="s">
@@ -12072,7 +13863,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W49">
-        <f>$C$3/U49</f>
+        <f t="shared" si="4"/>
         <v>36.071038251366119</v>
       </c>
     </row>
@@ -12093,7 +13884,7 @@
         <v>5.8796299999999997</v>
       </c>
       <c r="G50">
-        <f>$C$3/E50</f>
+        <f t="shared" si="0"/>
         <v>146.6888888888889</v>
       </c>
       <c r="J50" t="s">
@@ -12112,7 +13903,7 @@
         <v>22.222221999999999</v>
       </c>
       <c r="O50">
-        <f>$C$3/M50</f>
+        <f t="shared" si="3"/>
         <v>227.62068965517241</v>
       </c>
       <c r="R50" t="s">
@@ -12131,7 +13922,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W50">
-        <f>$C$3/U50</f>
+        <f t="shared" si="4"/>
         <v>36.469613259668506</v>
       </c>
     </row>
@@ -12152,7 +13943,7 @@
         <v>9.6759260000000005</v>
       </c>
       <c r="G51">
-        <f t="shared" ref="G51:G55" si="0">$C$3/E51</f>
+        <f t="shared" ref="G51:G55" si="5">$C$3/E51</f>
         <v>161</v>
       </c>
       <c r="J51" t="s">
@@ -12171,7 +13962,7 @@
         <v>0</v>
       </c>
       <c r="O51">
-        <f>$C$3/M51</f>
+        <f t="shared" si="3"/>
         <v>1.6804989816700611</v>
       </c>
       <c r="R51" t="s">
@@ -12190,7 +13981,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W51">
-        <f>$C$3/U51</f>
+        <f t="shared" si="4"/>
         <v>36.672222222222224</v>
       </c>
     </row>
@@ -12211,7 +14002,7 @@
         <v>11.898148000000001</v>
       </c>
       <c r="G52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>173.71052631578948</v>
       </c>
       <c r="J52" t="s">
@@ -12230,7 +14021,7 @@
         <v>0</v>
       </c>
       <c r="O52">
-        <f>$C$3/M52</f>
+        <f t="shared" si="3"/>
         <v>2.0506368437402922</v>
       </c>
       <c r="R52" t="s">
@@ -12249,7 +14040,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W52">
-        <f>$C$3/U52</f>
+        <f t="shared" si="4"/>
         <v>39.526946107784433</v>
       </c>
     </row>
@@ -12270,7 +14061,7 @@
         <v>16.666667</v>
       </c>
       <c r="G53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>200.03030303030303</v>
       </c>
       <c r="J53" t="s">
@@ -12289,7 +14080,7 @@
         <v>0</v>
       </c>
       <c r="O53">
-        <f>$C$3/M53</f>
+        <f t="shared" si="3"/>
         <v>2.5704828660436139</v>
       </c>
       <c r="R53" t="s">
@@ -12308,7 +14099,7 @@
         <v>1.8981479999999999</v>
       </c>
       <c r="W53">
-        <f>$C$3/U53</f>
+        <f t="shared" si="4"/>
         <v>40.006060606060608</v>
       </c>
     </row>
@@ -12329,7 +14120,7 @@
         <v>32.222222000000002</v>
       </c>
       <c r="G54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>264.04000000000002</v>
       </c>
       <c r="J54" t="s">
@@ -12348,7 +14139,7 @@
         <v>0</v>
       </c>
       <c r="O54">
-        <f>$C$3/M54</f>
+        <f t="shared" si="3"/>
         <v>3.3764705882352941</v>
       </c>
       <c r="R54" t="s">
@@ -12367,7 +14158,7 @@
         <v>1.8981479999999999</v>
       </c>
       <c r="W54">
-        <f>$C$3/U54</f>
+        <f t="shared" si="4"/>
         <v>40.25</v>
       </c>
     </row>
@@ -12388,7 +14179,7 @@
         <v>37.314815000000003</v>
       </c>
       <c r="G55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>300.04545454545456</v>
       </c>
       <c r="J55" t="s">
@@ -12407,7 +14198,7 @@
         <v>0</v>
       </c>
       <c r="O55">
-        <f>$C$3/M55</f>
+        <f t="shared" si="3"/>
         <v>4.661723163841808</v>
       </c>
       <c r="R55" t="s">
@@ -12426,7 +14217,7 @@
         <v>1.8981479999999999</v>
       </c>
       <c r="W55">
-        <f>$C$3/U55</f>
+        <f t="shared" si="4"/>
         <v>41.256250000000001</v>
       </c>
     </row>
@@ -12447,7 +14238,7 @@
         <v>0</v>
       </c>
       <c r="G56">
-        <f>$C$3/E56</f>
+        <f t="shared" ref="G56:G80" si="6">$C$3/E56</f>
         <v>1.2012738853503184</v>
       </c>
       <c r="J56" t="s">
@@ -12466,7 +14257,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O56">
-        <f>$C$3/M56</f>
+        <f t="shared" si="3"/>
         <v>6.640845070422535</v>
       </c>
       <c r="R56" t="s">
@@ -12485,7 +14276,7 @@
         <v>2.2222219999999999</v>
       </c>
       <c r="W56">
-        <f>$C$3/U56</f>
+        <f t="shared" si="4"/>
         <v>42.044585987261144</v>
       </c>
     </row>
@@ -12506,7 +14297,7 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <f>$C$3/E57</f>
+        <f t="shared" si="6"/>
         <v>1.3529411764705883</v>
       </c>
       <c r="J57" t="s">
@@ -12525,7 +14316,7 @@
         <v>0</v>
       </c>
       <c r="O57">
-        <f>$C$3/M57</f>
+        <f t="shared" si="3"/>
         <v>9.5805515239477508</v>
       </c>
       <c r="R57" t="s">
@@ -12544,7 +14335,7 @@
         <v>2.5462959999999999</v>
       </c>
       <c r="W57">
-        <f>$C$3/U57</f>
+        <f t="shared" si="4"/>
         <v>42.863636363636367</v>
       </c>
     </row>
@@ -12565,7 +14356,7 @@
         <v>0</v>
       </c>
       <c r="G58">
-        <f>$C$3/E58</f>
+        <f t="shared" si="6"/>
         <v>1.5557388640113128</v>
       </c>
       <c r="J58" t="s">
@@ -12584,7 +14375,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O58">
-        <f>$C$3/M58</f>
+        <f t="shared" si="3"/>
         <v>13.838574423480084</v>
       </c>
       <c r="R58" t="s">
@@ -12603,7 +14394,7 @@
         <v>2.2222219999999999</v>
       </c>
       <c r="W58">
-        <f>$C$3/U58</f>
+        <f t="shared" si="4"/>
         <v>43.143790849673202</v>
       </c>
     </row>
@@ -12624,7 +14415,7 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <f>$C$3/E59</f>
+        <f t="shared" si="6"/>
         <v>1.8485018202184262</v>
       </c>
       <c r="J59" t="s">
@@ -12643,7 +14434,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O59">
-        <f>$C$3/M59</f>
+        <f t="shared" si="3"/>
         <v>20.125</v>
       </c>
       <c r="R59" t="s">
@@ -12662,7 +14453,7 @@
         <v>3.0092590000000001</v>
       </c>
       <c r="W59">
-        <f>$C$3/U59</f>
+        <f t="shared" si="4"/>
         <v>43.143790849673202</v>
       </c>
     </row>
@@ -12683,7 +14474,7 @@
         <v>0</v>
       </c>
       <c r="G60">
-        <f>$C$3/E60</f>
+        <f t="shared" si="6"/>
         <v>2.292013888888889</v>
       </c>
       <c r="J60" t="s">
@@ -12702,7 +14493,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O60">
-        <f>$C$3/M60</f>
+        <f t="shared" si="3"/>
         <v>27.735294117647058</v>
       </c>
       <c r="R60" t="s">
@@ -12721,7 +14512,7 @@
         <v>1.8981479999999999</v>
       </c>
       <c r="W60">
-        <f>$C$3/U60</f>
+        <f t="shared" si="4"/>
         <v>43.715231788079471</v>
       </c>
     </row>
@@ -12742,7 +14533,7 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <f>$C$3/E61</f>
+        <f t="shared" si="6"/>
         <v>3.0419354838709678</v>
       </c>
       <c r="J61" t="s">
@@ -12761,7 +14552,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O61">
-        <f>$C$3/M61</f>
+        <f t="shared" si="3"/>
         <v>36.469613259668506</v>
       </c>
       <c r="R61" t="s">
@@ -12780,7 +14571,7 @@
         <v>2.2222219999999999</v>
       </c>
       <c r="W61">
-        <f>$C$3/U61</f>
+        <f t="shared" si="4"/>
         <v>44.302013422818789</v>
       </c>
     </row>
@@ -12801,7 +14592,7 @@
         <v>0</v>
       </c>
       <c r="G62">
-        <f>$C$3/E62</f>
+        <f t="shared" si="6"/>
         <v>4.4036024016010673</v>
       </c>
       <c r="J62" t="s">
@@ -12820,7 +14611,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="O62">
-        <f>$C$3/M62</f>
+        <f t="shared" si="3"/>
         <v>46.485915492957744</v>
       </c>
       <c r="R62" t="s">
@@ -12839,7 +14630,7 @@
         <v>2.2222219999999999</v>
       </c>
       <c r="W62">
-        <f>$C$3/U62</f>
+        <f t="shared" si="4"/>
         <v>45.212328767123289</v>
       </c>
     </row>
@@ -12860,7 +14651,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="G63">
-        <f>$C$3/E63</f>
+        <f t="shared" si="6"/>
         <v>6.8688865764828302</v>
       </c>
       <c r="J63" t="s">
@@ -12879,7 +14670,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="O63">
-        <f>$C$3/M63</f>
+        <f t="shared" si="3"/>
         <v>58.415929203539825</v>
       </c>
       <c r="R63" t="s">
@@ -12898,7 +14689,7 @@
         <v>3.3333330000000001</v>
       </c>
       <c r="W63">
-        <f>$C$3/U63</f>
+        <f t="shared" si="4"/>
         <v>46.16083916083916</v>
       </c>
     </row>
@@ -12919,7 +14710,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="G64">
-        <f>$C$3/E64</f>
+        <f t="shared" si="6"/>
         <v>10.62962962962963</v>
       </c>
       <c r="J64" t="s">
@@ -12938,7 +14729,7 @@
         <v>2.0833330000000001</v>
       </c>
       <c r="O64">
-        <f>$C$3/M64</f>
+        <f t="shared" si="3"/>
         <v>72.538461538461533</v>
       </c>
       <c r="R64" t="s">
@@ -12957,7 +14748,7 @@
         <v>3.6574070000000001</v>
       </c>
       <c r="W64">
-        <f>$C$3/U64</f>
+        <f t="shared" si="4"/>
         <v>46.815602836879435</v>
       </c>
     </row>
@@ -12978,7 +14769,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="G65">
-        <f>$C$3/E65</f>
+        <f t="shared" si="6"/>
         <v>15.531764705882352</v>
       </c>
       <c r="J65" t="s">
@@ -12997,7 +14788,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="O65">
-        <f>$C$3/M65</f>
+        <f t="shared" si="3"/>
         <v>88.013333333333335</v>
       </c>
       <c r="R65" t="s">
@@ -13016,7 +14807,7 @@
         <v>4.1203700000000003</v>
       </c>
       <c r="W65">
-        <f>$C$3/U65</f>
+        <f t="shared" si="4"/>
         <v>46.815602836879435</v>
       </c>
     </row>
@@ -13037,7 +14828,7 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <f>$C$3/E66</f>
+        <f t="shared" si="6"/>
         <v>21.431818181818183</v>
       </c>
       <c r="J66" t="s">
@@ -13056,7 +14847,7 @@
         <v>2.5462959999999999</v>
       </c>
       <c r="O66">
-        <f>$C$3/M66</f>
+        <f t="shared" si="3"/>
         <v>106.46774193548387</v>
       </c>
       <c r="R66" t="s">
@@ -13075,7 +14866,7 @@
         <v>4.7685190000000004</v>
       </c>
       <c r="W66">
-        <f>$C$3/U66</f>
+        <f t="shared" si="4"/>
         <v>47.489208633093526</v>
       </c>
     </row>
@@ -13096,7 +14887,7 @@
         <v>0.64814799999999995</v>
       </c>
       <c r="G67">
-        <f>$C$3/E67</f>
+        <f t="shared" si="6"/>
         <v>29.734234234234233</v>
       </c>
       <c r="J67" t="s">
@@ -13115,7 +14906,7 @@
         <v>4.4444439999999998</v>
       </c>
       <c r="O67">
-        <f>$C$3/M67</f>
+        <f t="shared" si="3"/>
         <v>129.43137254901961</v>
       </c>
       <c r="R67" t="s">
@@ -13134,7 +14925,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W67">
-        <f>$C$3/U67</f>
+        <f t="shared" si="4"/>
         <v>6.6879432624113475</v>
       </c>
     </row>
@@ -13155,7 +14946,7 @@
         <v>0.64814799999999995</v>
       </c>
       <c r="G68">
-        <f>$C$3/E68</f>
+        <f t="shared" si="6"/>
         <v>39.765060240963855</v>
       </c>
       <c r="J68" t="s">
@@ -13174,7 +14965,7 @@
         <v>8.1018519999999992</v>
       </c>
       <c r="O68">
-        <f>$C$3/M68</f>
+        <f t="shared" si="3"/>
         <v>157.16666666666666</v>
       </c>
       <c r="R68" t="s">
@@ -13193,7 +14984,7 @@
         <v>0</v>
       </c>
       <c r="W68">
-        <f>$C$3/U68</f>
+        <f t="shared" si="4"/>
         <v>6.7151576805696847</v>
       </c>
     </row>
@@ -13214,7 +15005,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="G69">
-        <f>$C$3/E69</f>
+        <f t="shared" si="6"/>
         <v>51.976377952755904</v>
       </c>
       <c r="J69" t="s">
@@ -13233,7 +15024,7 @@
         <v>11.898148000000001</v>
       </c>
       <c r="O69">
-        <f>$C$3/M69</f>
+        <f t="shared" ref="O69:O75" si="7">$C$3/M69</f>
         <v>188.6</v>
       </c>
       <c r="R69" t="s">
@@ -13252,7 +15043,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W69">
-        <f>$C$3/U69</f>
+        <f t="shared" ref="W69:W97" si="8">$C$3/U69</f>
         <v>10.444620253164556</v>
       </c>
     </row>
@@ -13273,7 +15064,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="G70">
-        <f>$C$3/E70</f>
+        <f t="shared" si="6"/>
         <v>64.715686274509807</v>
       </c>
       <c r="J70" t="s">
@@ -13292,7 +15083,7 @@
         <v>22.222221999999999</v>
       </c>
       <c r="O70">
-        <f>$C$3/M70</f>
+        <f t="shared" si="7"/>
         <v>227.62068965517241</v>
       </c>
       <c r="R70" t="s">
@@ -13311,7 +15102,7 @@
         <v>0.32407399999999997</v>
       </c>
       <c r="W70">
-        <f>$C$3/U70</f>
+        <f t="shared" si="8"/>
         <v>13.498977505112475</v>
       </c>
     </row>
@@ -13332,7 +15123,7 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="G71">
-        <f>$C$3/E71</f>
+        <f t="shared" si="6"/>
         <v>77.658823529411762</v>
       </c>
       <c r="J71" t="s">
@@ -13351,7 +15142,7 @@
         <v>31.435185000000001</v>
       </c>
       <c r="O71">
-        <f>$C$3/M71</f>
+        <f t="shared" si="7"/>
         <v>275.04166666666669</v>
       </c>
       <c r="R71" t="s">
@@ -13370,7 +15161,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W71">
-        <f>$C$3/U71</f>
+        <f t="shared" si="8"/>
         <v>17.555851063829788</v>
       </c>
     </row>
@@ -13391,7 +15182,7 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="G72">
-        <f>$C$3/E72</f>
+        <f t="shared" si="6"/>
         <v>92.971830985915489</v>
       </c>
       <c r="J72" t="s">
@@ -13410,7 +15201,7 @@
         <v>42.546295999999998</v>
       </c>
       <c r="O72">
-        <f>$C$3/M72</f>
+        <f t="shared" si="7"/>
         <v>330.05</v>
       </c>
       <c r="R72" t="s">
@@ -13429,7 +15220,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W72">
-        <f>$C$3/U72</f>
+        <f t="shared" si="8"/>
         <v>21.930232558139537</v>
       </c>
     </row>
@@ -13450,7 +15241,7 @@
         <v>3.6574070000000001</v>
       </c>
       <c r="G73">
-        <f>$C$3/E73</f>
+        <f t="shared" si="6"/>
         <v>110.01666666666667</v>
       </c>
       <c r="J73" t="s">
@@ -13469,7 +15260,7 @@
         <v>53.657406999999999</v>
       </c>
       <c r="O73">
-        <f>$C$3/M73</f>
+        <f t="shared" si="7"/>
         <v>366.72222222222223</v>
       </c>
       <c r="R73" t="s">
@@ -13488,7 +15279,7 @@
         <v>1.111111</v>
       </c>
       <c r="W73">
-        <f>$C$3/U73</f>
+        <f t="shared" si="8"/>
         <v>25.003787878787879</v>
       </c>
     </row>
@@ -13509,7 +15300,7 @@
         <v>3.7962959999999999</v>
       </c>
       <c r="G74">
-        <f>$C$3/E74</f>
+        <f t="shared" si="6"/>
         <v>132.02000000000001</v>
       </c>
       <c r="J74" t="s">
@@ -13528,7 +15319,7 @@
         <v>66.203704000000002</v>
       </c>
       <c r="O74">
-        <f>$C$3/M74</f>
+        <f t="shared" si="7"/>
         <v>412.5625</v>
       </c>
       <c r="R74" t="s">
@@ -13547,7 +15338,7 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="W74">
-        <f>$C$3/U74</f>
+        <f t="shared" si="8"/>
         <v>27.390041493775932</v>
       </c>
     </row>
@@ -13568,7 +15359,7 @@
         <v>7.4537040000000001</v>
       </c>
       <c r="G75">
-        <f>$C$3/E75</f>
+        <f t="shared" si="6"/>
         <v>157.16666666666666</v>
       </c>
       <c r="J75" t="s">
@@ -13587,7 +15378,7 @@
         <v>69.212963000000002</v>
       </c>
       <c r="O75">
-        <f>$C$3/M75</f>
+        <f t="shared" si="7"/>
         <v>440.06666666666666</v>
       </c>
       <c r="R75" t="s">
@@ -13606,7 +15397,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="W75">
-        <f>$C$3/U75</f>
+        <f t="shared" si="8"/>
         <v>28.20940170940171</v>
       </c>
     </row>
@@ -13627,7 +15418,7 @@
         <v>13.333333</v>
       </c>
       <c r="G76">
-        <f>$C$3/E76</f>
+        <f t="shared" si="6"/>
         <v>183.36111111111111</v>
       </c>
       <c r="R76" t="s">
@@ -13646,7 +15437,7 @@
         <v>1.4351849999999999</v>
       </c>
       <c r="W76">
-        <f>$C$3/U76</f>
+        <f t="shared" si="8"/>
         <v>31.433333333333334</v>
       </c>
     </row>
@@ -13667,7 +15458,7 @@
         <v>20.462962999999998</v>
       </c>
       <c r="G77">
-        <f>$C$3/E77</f>
+        <f t="shared" si="6"/>
         <v>212.93548387096774</v>
       </c>
       <c r="R77" t="s">
@@ -13686,7 +15477,7 @@
         <v>1.7592589999999999</v>
       </c>
       <c r="W77">
-        <f>$C$3/U77</f>
+        <f t="shared" si="8"/>
         <v>31.433333333333334</v>
       </c>
     </row>
@@ -13707,7 +15498,7 @@
         <v>28.101852000000001</v>
       </c>
       <c r="G78">
-        <f>$C$3/E78</f>
+        <f t="shared" si="6"/>
         <v>244.4814814814815</v>
       </c>
       <c r="R78" t="s">
@@ -13726,7 +15517,7 @@
         <v>1.8981479999999999</v>
       </c>
       <c r="W78">
-        <f>$C$3/U78</f>
+        <f t="shared" si="8"/>
         <v>32.517241379310342</v>
       </c>
     </row>
@@ -13747,7 +15538,7 @@
         <v>34.120370000000001</v>
       </c>
       <c r="G79">
-        <f>$C$3/E79</f>
+        <f t="shared" si="6"/>
         <v>287</v>
       </c>
       <c r="R79" t="s">
@@ -13766,7 +15557,7 @@
         <v>2.2222219999999999</v>
       </c>
       <c r="W79">
-        <f>$C$3/U79</f>
+        <f t="shared" si="8"/>
         <v>35.681081081081082</v>
       </c>
     </row>
@@ -13787,7 +15578,7 @@
         <v>41.435184999999997</v>
       </c>
       <c r="G80">
-        <f>$C$3/E80</f>
+        <f t="shared" si="6"/>
         <v>330.05</v>
       </c>
       <c r="R80" t="s">
@@ -13806,7 +15597,7 @@
         <v>2.5462959999999999</v>
       </c>
       <c r="W80">
-        <f>$C$3/U80</f>
+        <f t="shared" si="8"/>
         <v>36.071038251366119</v>
       </c>
     </row>
@@ -13827,7 +15618,7 @@
         <v>3.0092590000000001</v>
       </c>
       <c r="W81">
-        <f>$C$3/U81</f>
+        <f t="shared" si="8"/>
         <v>36.469613259668506</v>
       </c>
     </row>
@@ -13848,7 +15639,7 @@
         <v>2.8703699999999999</v>
       </c>
       <c r="W82">
-        <f>$C$3/U82</f>
+        <f t="shared" si="8"/>
         <v>37.084269662921351</v>
       </c>
     </row>
@@ -13869,7 +15660,7 @@
         <v>3.6574070000000001</v>
       </c>
       <c r="W83">
-        <f>$C$3/U83</f>
+        <f t="shared" si="8"/>
         <v>40.25</v>
       </c>
     </row>
@@ -13890,7 +15681,7 @@
         <v>4.4444439999999998</v>
       </c>
       <c r="W84">
-        <f>$C$3/U84</f>
+        <f t="shared" si="8"/>
         <v>40.25</v>
       </c>
     </row>
@@ -13911,7 +15702,7 @@
         <v>3.3333330000000001</v>
       </c>
       <c r="W85">
-        <f>$C$3/U85</f>
+        <f t="shared" si="8"/>
         <v>41</v>
       </c>
     </row>
@@ -13932,7 +15723,7 @@
         <v>4.1203700000000003</v>
       </c>
       <c r="W86">
-        <f>$C$3/U86</f>
+        <f t="shared" si="8"/>
         <v>42.044585987261144</v>
       </c>
     </row>
@@ -13953,7 +15744,7 @@
         <v>4.1203700000000003</v>
       </c>
       <c r="W87">
-        <f>$C$3/U87</f>
+        <f t="shared" si="8"/>
         <v>42.863636363636367</v>
       </c>
     </row>
@@ -13974,7 +15765,7 @@
         <v>7.4537040000000001</v>
       </c>
       <c r="W88">
-        <f>$C$3/U88</f>
+        <f t="shared" si="8"/>
         <v>43.143790849673202</v>
       </c>
     </row>
@@ -13995,7 +15786,7 @@
         <v>5.8796299999999997</v>
       </c>
       <c r="W89">
-        <f>$C$3/U89</f>
+        <f t="shared" si="8"/>
         <v>43.42763157894737</v>
       </c>
     </row>
@@ -14016,7 +15807,7 @@
         <v>4.9074070000000001</v>
       </c>
       <c r="W90">
-        <f>$C$3/U90</f>
+        <f t="shared" si="8"/>
         <v>44.006666666666668</v>
       </c>
     </row>
@@ -14037,7 +15828,7 @@
         <v>5.2314809999999996</v>
       </c>
       <c r="W91">
-        <f>$C$3/U91</f>
+        <f t="shared" si="8"/>
         <v>44.601351351351354</v>
       </c>
     </row>
@@ -14058,7 +15849,7 @@
         <v>4.1203700000000003</v>
       </c>
       <c r="W92">
-        <f>$C$3/U92</f>
+        <f t="shared" si="8"/>
         <v>45.524137931034481</v>
       </c>
     </row>
@@ -14079,7 +15870,7 @@
         <v>5.2314809999999996</v>
       </c>
       <c r="W93">
-        <f>$C$3/U93</f>
+        <f t="shared" si="8"/>
         <v>46.16083916083916</v>
       </c>
     </row>
@@ -14100,7 +15891,7 @@
         <v>7.3148150000000003</v>
       </c>
       <c r="W94">
-        <f>$C$3/U94</f>
+        <f t="shared" si="8"/>
         <v>47.15</v>
       </c>
     </row>
@@ -14121,7 +15912,7 @@
         <v>7.3148150000000003</v>
       </c>
       <c r="W95">
-        <f>$C$3/U95</f>
+        <f t="shared" si="8"/>
         <v>48.182481751824817</v>
       </c>
     </row>
@@ -14142,7 +15933,7 @@
         <v>6.9907409999999999</v>
       </c>
       <c r="W96">
-        <f>$C$3/U96</f>
+        <f t="shared" si="8"/>
         <v>48.182481751824817</v>
       </c>
     </row>
@@ -14163,14 +15954,14 @@
         <v>8.1018519999999992</v>
       </c>
       <c r="W97">
-        <f>$C$3/U97</f>
+        <f t="shared" si="8"/>
         <v>48.896296296296299</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="R5:W103">
-    <sortCondition ref="T5:T103"/>
-    <sortCondition ref="W5:W103"/>
+  <sortState ref="Z5:AD32">
+    <sortCondition ref="AD5:AD32"/>
+    <sortCondition ref="AA5:AA32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>